<commit_message>
Ajout groupe sur IMS
</commit_message>
<xml_diff>
--- a/back/scriptImport/mtp_data.xlsx
+++ b/back/scriptImport/mtp_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\EstyaTicketing\back\scriptImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5683ED-55E8-44B3-A705-1CC974F51320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1ED703-E67D-468C-BBE5-9B0BF54FD9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3099,9 +3099,6 @@
     <t>BTS CG 1 A - ESTYA Montpellier</t>
   </si>
   <si>
-    <t>RNCP DWWM 1 A - ESTYA Montpellier</t>
-  </si>
-  <si>
     <t>BTS SIO 1 A - ESTYA Montpellier</t>
   </si>
   <si>
@@ -3120,9 +3117,6 @@
     <t>RNCP MPI - Cybersécurité 1 A - ESTYA Montpellier</t>
   </si>
   <si>
-    <t>RNCP MRH 1 A - ESTYA Montpellier</t>
-  </si>
-  <si>
     <t>BTS MCO 2 A - ESTYA Montpellier</t>
   </si>
   <si>
@@ -3132,12 +3126,6 @@
     <t>RNCP NTC 2 A - ESTYA Montpellier</t>
   </si>
   <si>
-    <t>RNCP TSSR 2 A - ESTYA Montpellier</t>
-  </si>
-  <si>
-    <t>RNCP DWWM 2 A - ESTYA Montpellier</t>
-  </si>
-  <si>
     <t>BIM Mod 2 A - ESTYA Montpellier</t>
   </si>
   <si>
@@ -3150,9 +3138,6 @@
     <t>RNCP MPI - Cybersécurité 2 A - ESTYA Montpellier</t>
   </si>
   <si>
-    <t>RNCP MRH 2 A - ESTYA Montpellier</t>
-  </si>
-  <si>
     <t>CDMC 1 A - ESTYA Montpellier</t>
   </si>
   <si>
@@ -3172,6 +3157,21 @@
   </si>
   <si>
     <t>2022 - 2023</t>
+  </si>
+  <si>
+    <t>RNCP DWWM  1 A - ESTYA Montpellier</t>
+  </si>
+  <si>
+    <t>RNCP MRH  1 A - ESTYA Montpellier</t>
+  </si>
+  <si>
+    <t>RNCP TSSR  2 A - ESTYA Montpellier</t>
+  </si>
+  <si>
+    <t>RNCP DWWM  2 A - ESTYA Montpellier</t>
+  </si>
+  <si>
+    <t>RNCP MRH  2 A - ESTYA Montpellier</t>
   </si>
 </sst>
 </file>
@@ -3315,7 +3315,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -3345,6 +3345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{3DB7AE96-F838-44EC-825F-7DEE146B208A}"/>
@@ -3983,8 +3984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="G221" sqref="G221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4037,7 +4038,7 @@
         <v>1021</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>1047</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -4078,7 +4079,7 @@
         <v>9</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -4119,7 +4120,7 @@
         <v>9</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -4160,7 +4161,7 @@
         <v>23</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -4201,7 +4202,7 @@
         <v>9</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -4242,7 +4243,7 @@
         <v>9</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -4283,7 +4284,7 @@
         <v>9</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -4324,7 +4325,7 @@
         <v>9</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -4365,7 +4366,7 @@
         <v>9</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -4406,7 +4407,7 @@
         <v>9</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -4447,7 +4448,7 @@
         <v>9</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -4488,7 +4489,7 @@
         <v>9</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -4519,7 +4520,7 @@
       <c r="I13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="18" t="s">
         <v>69</v>
       </c>
       <c r="K13" s="1" t="s">
@@ -4529,7 +4530,7 @@
         <v>9</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -4570,7 +4571,7 @@
         <v>9</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -4611,7 +4612,7 @@
         <v>9</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -4652,7 +4653,7 @@
         <v>9</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -4693,7 +4694,7 @@
         <v>9</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -4734,7 +4735,7 @@
         <v>9</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -4775,7 +4776,7 @@
         <v>9</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -4806,7 +4807,7 @@
       <c r="I20" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="18" t="s">
         <v>108</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -4816,7 +4817,7 @@
         <v>9</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -4857,7 +4858,7 @@
         <v>9</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -4898,7 +4899,7 @@
         <v>9</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -4939,7 +4940,7 @@
         <v>9</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -4980,7 +4981,7 @@
         <v>9</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -5021,7 +5022,7 @@
         <v>9</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -5062,7 +5063,7 @@
         <v>9</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -5103,7 +5104,7 @@
         <v>9</v>
       </c>
       <c r="M27" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -5144,7 +5145,7 @@
         <v>9</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -5185,7 +5186,7 @@
         <v>9</v>
       </c>
       <c r="M29" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -5226,7 +5227,7 @@
         <v>9</v>
       </c>
       <c r="M30" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -5257,7 +5258,7 @@
       <c r="I31" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="J31" s="18" t="s">
         <v>166</v>
       </c>
       <c r="K31" s="1" t="s">
@@ -5267,7 +5268,7 @@
         <v>9</v>
       </c>
       <c r="M31" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -5308,7 +5309,7 @@
         <v>9</v>
       </c>
       <c r="M32" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -5349,7 +5350,7 @@
         <v>9</v>
       </c>
       <c r="M33" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -5390,7 +5391,7 @@
         <v>9</v>
       </c>
       <c r="M34" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -5431,7 +5432,7 @@
         <v>9</v>
       </c>
       <c r="M35" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -5454,7 +5455,7 @@
         <v>191</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>1024</v>
+        <v>1044</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>46</v>
@@ -5472,7 +5473,7 @@
         <v>9</v>
       </c>
       <c r="M36" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -5495,7 +5496,7 @@
         <v>191</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>1024</v>
+        <v>1044</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>46</v>
@@ -5503,7 +5504,7 @@
       <c r="I37" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="J37" s="9" t="s">
+      <c r="J37" s="19" t="s">
         <v>198</v>
       </c>
       <c r="K37" s="1" t="s">
@@ -5513,7 +5514,7 @@
         <v>23</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -5536,7 +5537,7 @@
         <v>202</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>106</v>
@@ -5554,7 +5555,7 @@
         <v>9</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -5577,7 +5578,7 @@
         <v>202</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>46</v>
@@ -5595,7 +5596,7 @@
         <v>9</v>
       </c>
       <c r="M39" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -5618,7 +5619,7 @@
         <v>202</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>46</v>
@@ -5636,7 +5637,7 @@
         <v>9</v>
       </c>
       <c r="M40" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -5659,7 +5660,7 @@
         <v>202</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>46</v>
@@ -5677,7 +5678,7 @@
         <v>9</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -5700,7 +5701,7 @@
         <v>202</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>46</v>
@@ -5708,7 +5709,7 @@
       <c r="I42" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J42" s="18" t="s">
         <v>223</v>
       </c>
       <c r="K42" s="1" t="s">
@@ -5718,7 +5719,7 @@
         <v>9</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -5741,7 +5742,7 @@
         <v>202</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>180</v>
@@ -5759,7 +5760,7 @@
         <v>9</v>
       </c>
       <c r="M43" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -5782,7 +5783,7 @@
         <v>202</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>79</v>
@@ -5800,7 +5801,7 @@
         <v>9</v>
       </c>
       <c r="M44" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -5823,7 +5824,7 @@
         <v>202</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>14</v>
@@ -5841,7 +5842,7 @@
         <v>9</v>
       </c>
       <c r="M45" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -5864,7 +5865,7 @@
         <v>202</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>14</v>
@@ -5882,7 +5883,7 @@
         <v>9</v>
       </c>
       <c r="M46" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -5905,7 +5906,7 @@
         <v>202</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>14</v>
@@ -5923,7 +5924,7 @@
         <v>9</v>
       </c>
       <c r="M47" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -5946,7 +5947,7 @@
         <v>202</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
@@ -5964,7 +5965,7 @@
         <v>9</v>
       </c>
       <c r="M48" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -5987,7 +5988,7 @@
         <v>202</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>79</v>
@@ -6005,7 +6006,7 @@
         <v>9</v>
       </c>
       <c r="M49" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -6028,7 +6029,7 @@
         <v>202</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
@@ -6046,7 +6047,7 @@
         <v>9</v>
       </c>
       <c r="M50" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -6069,7 +6070,7 @@
         <v>202</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>14</v>
@@ -6087,7 +6088,7 @@
         <v>9</v>
       </c>
       <c r="M51" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -6107,7 +6108,7 @@
         <v>202</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H52" s="9" t="s">
         <v>20</v>
@@ -6119,7 +6120,7 @@
         <v>9</v>
       </c>
       <c r="M52" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -6142,7 +6143,7 @@
         <v>202</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>14</v>
@@ -6160,7 +6161,7 @@
         <v>9</v>
       </c>
       <c r="M53" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -6183,7 +6184,7 @@
         <v>202</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>14</v>
@@ -6201,7 +6202,7 @@
         <v>9</v>
       </c>
       <c r="M54" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -6224,7 +6225,7 @@
         <v>202</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>14</v>
@@ -6242,7 +6243,7 @@
         <v>9</v>
       </c>
       <c r="M55" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -6265,7 +6266,7 @@
         <v>202</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="H56" s="9" t="s">
         <v>46</v>
@@ -6283,7 +6284,7 @@
         <v>9</v>
       </c>
       <c r="M56" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -6306,7 +6307,7 @@
         <v>294</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>14</v>
@@ -6324,7 +6325,7 @@
         <v>9</v>
       </c>
       <c r="M57" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -6347,7 +6348,7 @@
         <v>294</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>73</v>
@@ -6365,7 +6366,7 @@
         <v>9</v>
       </c>
       <c r="M58" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -6388,7 +6389,7 @@
         <v>294</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>14</v>
@@ -6406,7 +6407,7 @@
         <v>9</v>
       </c>
       <c r="M59" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -6429,7 +6430,7 @@
         <v>294</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>73</v>
@@ -6447,7 +6448,7 @@
         <v>9</v>
       </c>
       <c r="M60" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -6467,10 +6468,10 @@
         <v>314</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>20</v>
@@ -6488,7 +6489,7 @@
         <v>23</v>
       </c>
       <c r="M61" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -6508,10 +6509,10 @@
         <v>320</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>321</v>
@@ -6529,7 +6530,7 @@
         <v>9</v>
       </c>
       <c r="M62" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -6549,10 +6550,10 @@
         <v>326</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>327</v>
@@ -6570,7 +6571,7 @@
         <v>23</v>
       </c>
       <c r="M63" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -6590,10 +6591,10 @@
         <v>332</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>46</v>
@@ -6611,7 +6612,7 @@
         <v>9</v>
       </c>
       <c r="M64" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -6631,10 +6632,10 @@
         <v>337</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>338</v>
@@ -6652,7 +6653,7 @@
         <v>9</v>
       </c>
       <c r="M65" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -6672,10 +6673,10 @@
         <v>343</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>344</v>
@@ -6693,7 +6694,7 @@
         <v>23</v>
       </c>
       <c r="M66" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -6713,10 +6714,10 @@
         <v>349</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>79</v>
@@ -6734,7 +6735,7 @@
         <v>23</v>
       </c>
       <c r="M67" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -6754,10 +6755,10 @@
         <v>354</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>338</v>
@@ -6775,7 +6776,7 @@
         <v>9</v>
       </c>
       <c r="M68" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -6795,10 +6796,10 @@
         <v>359</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>338</v>
@@ -6816,7 +6817,7 @@
         <v>9</v>
       </c>
       <c r="M69" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -6836,10 +6837,10 @@
         <v>364</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>79</v>
@@ -6857,7 +6858,7 @@
         <v>23</v>
       </c>
       <c r="M70" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -6877,10 +6878,10 @@
         <v>369</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>73</v>
@@ -6898,7 +6899,7 @@
         <v>23</v>
       </c>
       <c r="M71" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -6918,10 +6919,10 @@
         <v>374</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>375</v>
@@ -6939,7 +6940,7 @@
         <v>9</v>
       </c>
       <c r="M72" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -6959,10 +6960,10 @@
         <v>380</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>381</v>
@@ -6980,7 +6981,7 @@
         <v>9</v>
       </c>
       <c r="M73" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -7000,10 +7001,10 @@
         <v>386</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>387</v>
@@ -7021,7 +7022,7 @@
         <v>9</v>
       </c>
       <c r="M74" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -7041,10 +7042,10 @@
         <v>392</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>85</v>
@@ -7062,7 +7063,7 @@
         <v>9</v>
       </c>
       <c r="M75" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -7082,10 +7083,10 @@
         <v>397</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>79</v>
@@ -7103,7 +7104,7 @@
         <v>23</v>
       </c>
       <c r="M76" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -7123,10 +7124,10 @@
         <v>401</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>79</v>
@@ -7144,7 +7145,7 @@
         <v>23</v>
       </c>
       <c r="M77" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -7164,10 +7165,10 @@
         <v>406</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>338</v>
@@ -7185,7 +7186,7 @@
         <v>9</v>
       </c>
       <c r="M78" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -7205,10 +7206,10 @@
         <v>411</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>79</v>
@@ -7226,7 +7227,7 @@
         <v>9</v>
       </c>
       <c r="M79" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -7246,10 +7247,10 @@
         <v>416</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>106</v>
@@ -7267,7 +7268,7 @@
         <v>23</v>
       </c>
       <c r="M80" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -7287,10 +7288,10 @@
         <v>421</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>46</v>
@@ -7308,7 +7309,7 @@
         <v>9</v>
       </c>
       <c r="M81" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -7328,10 +7329,10 @@
         <v>426</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>338</v>
@@ -7349,7 +7350,7 @@
         <v>9</v>
       </c>
       <c r="M82" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -7369,10 +7370,10 @@
         <v>431</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>14</v>
@@ -7390,7 +7391,7 @@
         <v>9</v>
       </c>
       <c r="M83" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -7410,10 +7411,10 @@
         <v>436</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>79</v>
@@ -7431,7 +7432,7 @@
         <v>23</v>
       </c>
       <c r="M84" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -7451,10 +7452,10 @@
         <v>441</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>73</v>
@@ -7472,7 +7473,7 @@
         <v>9</v>
       </c>
       <c r="M85" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -7492,10 +7493,10 @@
         <v>446</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>73</v>
@@ -7513,7 +7514,7 @@
         <v>23</v>
       </c>
       <c r="M86" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -7533,10 +7534,10 @@
         <v>451</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>452</v>
@@ -7554,7 +7555,7 @@
         <v>23</v>
       </c>
       <c r="M87" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -7574,10 +7575,10 @@
         <v>457</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>14</v>
@@ -7592,7 +7593,7 @@
         <v>9</v>
       </c>
       <c r="M88" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -7612,10 +7613,10 @@
         <v>461</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>73</v>
@@ -7633,7 +7634,7 @@
         <v>9</v>
       </c>
       <c r="M89" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -7653,10 +7654,10 @@
         <v>466</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H90" s="9" t="s">
         <v>73</v>
@@ -7674,7 +7675,7 @@
         <v>9</v>
       </c>
       <c r="M90" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -7694,10 +7695,10 @@
         <v>471</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>344</v>
@@ -7715,7 +7716,7 @@
         <v>9</v>
       </c>
       <c r="M91" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -7735,10 +7736,10 @@
         <v>477</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>46</v>
@@ -7756,7 +7757,7 @@
         <v>23</v>
       </c>
       <c r="M92" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -7776,10 +7777,10 @@
         <v>482</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>338</v>
@@ -7797,7 +7798,7 @@
         <v>9</v>
       </c>
       <c r="M93" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -7820,7 +7821,7 @@
         <v>488</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>381</v>
@@ -7838,7 +7839,7 @@
         <v>9</v>
       </c>
       <c r="M94" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -7861,7 +7862,7 @@
         <v>488</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>381</v>
@@ -7879,7 +7880,7 @@
         <v>23</v>
       </c>
       <c r="M95" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -7902,7 +7903,7 @@
         <v>498</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>14</v>
@@ -7920,7 +7921,7 @@
         <v>23</v>
       </c>
       <c r="M96" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -7943,7 +7944,7 @@
         <v>503</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>1031</v>
+        <v>1045</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>20</v>
@@ -7961,7 +7962,7 @@
         <v>23</v>
       </c>
       <c r="M97" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -7984,7 +7985,7 @@
         <v>503</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>1031</v>
+        <v>1045</v>
       </c>
       <c r="H98" s="9" t="s">
         <v>452</v>
@@ -8002,7 +8003,7 @@
         <v>23</v>
       </c>
       <c r="M98" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -8025,7 +8026,7 @@
         <v>4</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>52</v>
@@ -8043,7 +8044,7 @@
         <v>23</v>
       </c>
       <c r="M99" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -8066,7 +8067,7 @@
         <v>4</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>20</v>
@@ -8084,7 +8085,7 @@
         <v>23</v>
       </c>
       <c r="M100" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -8107,7 +8108,7 @@
         <v>4</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>73</v>
@@ -8125,7 +8126,7 @@
         <v>23</v>
       </c>
       <c r="M101" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -8148,7 +8149,7 @@
         <v>4</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>14</v>
@@ -8166,7 +8167,7 @@
         <v>23</v>
       </c>
       <c r="M102" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -8189,7 +8190,7 @@
         <v>4</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>528</v>
@@ -8207,7 +8208,7 @@
         <v>23</v>
       </c>
       <c r="M103" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -8230,7 +8231,7 @@
         <v>4</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>85</v>
@@ -8248,7 +8249,7 @@
         <v>23</v>
       </c>
       <c r="M104" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -8271,7 +8272,7 @@
         <v>4</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>14</v>
@@ -8289,7 +8290,7 @@
         <v>9</v>
       </c>
       <c r="M105" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -8312,7 +8313,7 @@
         <v>4</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="H106" s="9" t="s">
         <v>159</v>
@@ -8330,7 +8331,7 @@
         <v>23</v>
       </c>
       <c r="M106" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -8353,7 +8354,7 @@
         <v>4</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>14</v>
@@ -8371,7 +8372,7 @@
         <v>9</v>
       </c>
       <c r="M107" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -8394,7 +8395,7 @@
         <v>548</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>14</v>
@@ -8412,7 +8413,7 @@
         <v>9</v>
       </c>
       <c r="M108" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -8435,7 +8436,7 @@
         <v>548</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>73</v>
@@ -8453,7 +8454,7 @@
         <v>9</v>
       </c>
       <c r="M109" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -8476,7 +8477,7 @@
         <v>548</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>381</v>
@@ -8494,7 +8495,7 @@
         <v>9</v>
       </c>
       <c r="M110" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -8517,7 +8518,7 @@
         <v>548</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="H111" s="1" t="s">
         <v>73</v>
@@ -8535,7 +8536,7 @@
         <v>9</v>
       </c>
       <c r="M111" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -8558,7 +8559,7 @@
         <v>548</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>381</v>
@@ -8576,7 +8577,7 @@
         <v>23</v>
       </c>
       <c r="M112" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -8599,7 +8600,7 @@
         <v>548</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="H113" s="1" t="s">
         <v>327</v>
@@ -8617,7 +8618,7 @@
         <v>9</v>
       </c>
       <c r="M113" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -8640,7 +8641,7 @@
         <v>548</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="H114" s="9" t="s">
         <v>46</v>
@@ -8658,7 +8659,7 @@
         <v>23</v>
       </c>
       <c r="M114" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -8681,7 +8682,7 @@
         <v>577</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>375</v>
@@ -8699,7 +8700,7 @@
         <v>23</v>
       </c>
       <c r="M115" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -8722,7 +8723,7 @@
         <v>577</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>79</v>
@@ -8740,7 +8741,7 @@
         <v>9</v>
       </c>
       <c r="M116" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -8763,7 +8764,7 @@
         <v>577</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>73</v>
@@ -8781,7 +8782,7 @@
         <v>23</v>
       </c>
       <c r="M117" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -8804,7 +8805,7 @@
         <v>577</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>79</v>
@@ -8822,7 +8823,7 @@
         <v>23</v>
       </c>
       <c r="M118" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
@@ -8845,7 +8846,7 @@
         <v>577</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>73</v>
@@ -8863,7 +8864,7 @@
         <v>23</v>
       </c>
       <c r="M119" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
@@ -8886,7 +8887,7 @@
         <v>577</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>46</v>
@@ -8904,7 +8905,7 @@
         <v>23</v>
       </c>
       <c r="M120" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -8927,7 +8928,7 @@
         <v>577</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>73</v>
@@ -8945,7 +8946,7 @@
         <v>23</v>
       </c>
       <c r="M121" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
@@ -8968,7 +8969,7 @@
         <v>577</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>14</v>
@@ -8986,7 +8987,7 @@
         <v>9</v>
       </c>
       <c r="M122" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
@@ -9009,7 +9010,7 @@
         <v>577</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>79</v>
@@ -9027,7 +9028,7 @@
         <v>9</v>
       </c>
       <c r="M123" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -9050,7 +9051,7 @@
         <v>577</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H124" s="1" t="s">
         <v>614</v>
@@ -9068,7 +9069,7 @@
         <v>23</v>
       </c>
       <c r="M124" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
@@ -9091,7 +9092,7 @@
         <v>577</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>14</v>
@@ -9109,7 +9110,7 @@
         <v>23</v>
       </c>
       <c r="M125" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
@@ -9132,7 +9133,7 @@
         <v>577</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>14</v>
@@ -9150,7 +9151,7 @@
         <v>9</v>
       </c>
       <c r="M126" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
@@ -9173,7 +9174,7 @@
         <v>577</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>14</v>
@@ -9191,7 +9192,7 @@
         <v>23</v>
       </c>
       <c r="M127" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
@@ -9214,7 +9215,7 @@
         <v>577</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>52</v>
@@ -9232,7 +9233,7 @@
         <v>23</v>
       </c>
       <c r="M128" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
@@ -9255,7 +9256,7 @@
         <v>577</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H129" s="1" t="s">
         <v>79</v>
@@ -9267,7 +9268,7 @@
         <v>23</v>
       </c>
       <c r="M129" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
@@ -9290,7 +9291,7 @@
         <v>577</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H130" s="1" t="s">
         <v>73</v>
@@ -9308,7 +9309,7 @@
         <v>9</v>
       </c>
       <c r="M130" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
@@ -9331,7 +9332,7 @@
         <v>577</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H131" s="1" t="s">
         <v>46</v>
@@ -9349,7 +9350,7 @@
         <v>9</v>
       </c>
       <c r="M131" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
@@ -9372,7 +9373,7 @@
         <v>577</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>375</v>
@@ -9390,7 +9391,7 @@
         <v>9</v>
       </c>
       <c r="M132" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -9413,7 +9414,7 @@
         <v>577</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>79</v>
@@ -9431,7 +9432,7 @@
         <v>9</v>
       </c>
       <c r="M133" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -9454,7 +9455,7 @@
         <v>577</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="H134" s="9" t="s">
         <v>73</v>
@@ -9472,7 +9473,7 @@
         <v>9</v>
       </c>
       <c r="M134" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
@@ -9495,7 +9496,7 @@
         <v>656</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>1035</v>
+        <v>1046</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>73</v>
@@ -9513,7 +9514,7 @@
         <v>23</v>
       </c>
       <c r="M135" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
@@ -9536,7 +9537,7 @@
         <v>656</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>1035</v>
+        <v>1046</v>
       </c>
       <c r="H136" s="1" t="s">
         <v>14</v>
@@ -9554,7 +9555,7 @@
         <v>23</v>
       </c>
       <c r="M136" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -9577,7 +9578,7 @@
         <v>656</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>1035</v>
+        <v>1046</v>
       </c>
       <c r="H137" s="1" t="s">
         <v>14</v>
@@ -9595,7 +9596,7 @@
         <v>9</v>
       </c>
       <c r="M137" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
@@ -9618,7 +9619,7 @@
         <v>656</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>1035</v>
+        <v>1046</v>
       </c>
       <c r="H138" s="9" t="s">
         <v>73</v>
@@ -9636,7 +9637,7 @@
         <v>9</v>
       </c>
       <c r="M138" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
@@ -9659,7 +9660,7 @@
         <v>656</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>1035</v>
+        <v>1046</v>
       </c>
       <c r="H139" s="1" t="s">
         <v>73</v>
@@ -9677,7 +9678,7 @@
         <v>9</v>
       </c>
       <c r="M139" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
@@ -9700,7 +9701,7 @@
         <v>191</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="H140" s="1" t="s">
         <v>381</v>
@@ -9718,7 +9719,7 @@
         <v>23</v>
       </c>
       <c r="M140" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
@@ -9741,7 +9742,7 @@
         <v>191</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="H141" s="1" t="s">
         <v>381</v>
@@ -9759,7 +9760,7 @@
         <v>23</v>
       </c>
       <c r="M141" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
@@ -9782,7 +9783,7 @@
         <v>191</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="H142" s="1" t="s">
         <v>14</v>
@@ -9800,7 +9801,7 @@
         <v>9</v>
       </c>
       <c r="M142" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
@@ -9823,7 +9824,7 @@
         <v>191</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="H143" s="1" t="s">
         <v>79</v>
@@ -9841,7 +9842,7 @@
         <v>9</v>
       </c>
       <c r="M143" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
@@ -9864,7 +9865,7 @@
         <v>191</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="H144" s="1" t="s">
         <v>5</v>
@@ -9882,7 +9883,7 @@
         <v>9</v>
       </c>
       <c r="M144" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
@@ -9905,7 +9906,7 @@
         <v>191</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>79</v>
@@ -9923,7 +9924,7 @@
         <v>9</v>
       </c>
       <c r="M145" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
@@ -9946,7 +9947,7 @@
         <v>191</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>344</v>
@@ -9964,7 +9965,7 @@
         <v>23</v>
       </c>
       <c r="M146" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
@@ -9987,7 +9988,7 @@
         <v>191</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>180</v>
@@ -10005,7 +10006,7 @@
         <v>9</v>
       </c>
       <c r="M147" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
@@ -10028,7 +10029,7 @@
         <v>191</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>1036</v>
+        <v>1047</v>
       </c>
       <c r="H148" s="9" t="s">
         <v>79</v>
@@ -10046,7 +10047,7 @@
         <v>9</v>
       </c>
       <c r="M148" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
@@ -10069,7 +10070,7 @@
         <v>294</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="H149" s="1" t="s">
         <v>14</v>
@@ -10087,7 +10088,7 @@
         <v>9</v>
       </c>
       <c r="M149" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
@@ -10110,7 +10111,7 @@
         <v>294</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="H150" s="1" t="s">
         <v>79</v>
@@ -10128,7 +10129,7 @@
         <v>23</v>
       </c>
       <c r="M150" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
@@ -10151,7 +10152,7 @@
         <v>294</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="H151" s="1" t="s">
         <v>46</v>
@@ -10169,7 +10170,7 @@
         <v>23</v>
       </c>
       <c r="M151" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
@@ -10192,7 +10193,7 @@
         <v>294</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="H152" s="1" t="s">
         <v>14</v>
@@ -10210,7 +10211,7 @@
         <v>9</v>
       </c>
       <c r="M152" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
@@ -10233,7 +10234,7 @@
         <v>294</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="H153" s="1" t="s">
         <v>344</v>
@@ -10251,7 +10252,7 @@
         <v>9</v>
       </c>
       <c r="M153" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -10274,7 +10275,7 @@
         <v>294</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>452</v>
@@ -10292,7 +10293,7 @@
         <v>9</v>
       </c>
       <c r="M154" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
@@ -10315,7 +10316,7 @@
         <v>294</v>
       </c>
       <c r="G155" s="1" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="H155" s="9" t="s">
         <v>14</v>
@@ -10333,7 +10334,7 @@
         <v>9</v>
       </c>
       <c r="M155" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
@@ -10356,7 +10357,7 @@
         <v>315</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>381</v>
@@ -10374,7 +10375,7 @@
         <v>9</v>
       </c>
       <c r="M156" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
@@ -10397,7 +10398,7 @@
         <v>315</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H157" s="1" t="s">
         <v>338</v>
@@ -10415,7 +10416,7 @@
         <v>9</v>
       </c>
       <c r="M157" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
@@ -10438,7 +10439,7 @@
         <v>315</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>338</v>
@@ -10456,7 +10457,7 @@
         <v>23</v>
       </c>
       <c r="M158" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
@@ -10479,7 +10480,7 @@
         <v>315</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>14</v>
@@ -10497,7 +10498,7 @@
         <v>9</v>
       </c>
       <c r="M159" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
@@ -10520,7 +10521,7 @@
         <v>315</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>338</v>
@@ -10538,7 +10539,7 @@
         <v>23</v>
       </c>
       <c r="M160" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
@@ -10561,7 +10562,7 @@
         <v>315</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>79</v>
@@ -10579,7 +10580,7 @@
         <v>23</v>
       </c>
       <c r="M161" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
@@ -10602,7 +10603,7 @@
         <v>315</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>452</v>
@@ -10620,7 +10621,7 @@
         <v>9</v>
       </c>
       <c r="M162" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
@@ -10643,7 +10644,7 @@
         <v>315</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H163" s="1" t="s">
         <v>79</v>
@@ -10661,7 +10662,7 @@
         <v>23</v>
       </c>
       <c r="M163" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
@@ -10684,7 +10685,7 @@
         <v>315</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H164" s="1" t="s">
         <v>381</v>
@@ -10702,7 +10703,7 @@
         <v>23</v>
       </c>
       <c r="M164" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
@@ -10725,7 +10726,7 @@
         <v>315</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H165" s="1" t="s">
         <v>14</v>
@@ -10743,7 +10744,7 @@
         <v>9</v>
       </c>
       <c r="M165" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
@@ -10766,7 +10767,7 @@
         <v>315</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H166" s="1" t="s">
         <v>73</v>
@@ -10784,7 +10785,7 @@
         <v>23</v>
       </c>
       <c r="M166" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
@@ -10807,7 +10808,7 @@
         <v>315</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H167" s="1" t="s">
         <v>381</v>
@@ -10825,7 +10826,7 @@
         <v>23</v>
       </c>
       <c r="M167" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
@@ -10848,7 +10849,7 @@
         <v>315</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H168" s="1" t="s">
         <v>106</v>
@@ -10866,7 +10867,7 @@
         <v>9</v>
       </c>
       <c r="M168" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
@@ -10889,7 +10890,7 @@
         <v>315</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H169" s="1" t="s">
         <v>106</v>
@@ -10907,7 +10908,7 @@
         <v>23</v>
       </c>
       <c r="M169" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
@@ -10930,7 +10931,7 @@
         <v>315</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H170" s="1" t="s">
         <v>79</v>
@@ -10948,7 +10949,7 @@
         <v>9</v>
       </c>
       <c r="M170" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
@@ -10971,7 +10972,7 @@
         <v>315</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H171" s="1" t="s">
         <v>159</v>
@@ -10989,7 +10990,7 @@
         <v>9</v>
       </c>
       <c r="M171" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
@@ -11012,7 +11013,7 @@
         <v>315</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H172" s="1" t="s">
         <v>79</v>
@@ -11030,7 +11031,7 @@
         <v>23</v>
       </c>
       <c r="M172" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
@@ -11053,7 +11054,7 @@
         <v>315</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H173" s="1" t="s">
         <v>452</v>
@@ -11071,7 +11072,7 @@
         <v>23</v>
       </c>
       <c r="M173" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
@@ -11094,7 +11095,7 @@
         <v>315</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H174" s="1" t="s">
         <v>14</v>
@@ -11112,7 +11113,7 @@
         <v>9</v>
       </c>
       <c r="M174" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
@@ -11135,7 +11136,7 @@
         <v>315</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H175" s="1" t="s">
         <v>79</v>
@@ -11153,7 +11154,7 @@
         <v>9</v>
       </c>
       <c r="M175" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
@@ -11176,7 +11177,7 @@
         <v>315</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H176" s="1" t="s">
         <v>106</v>
@@ -11194,7 +11195,7 @@
         <v>23</v>
       </c>
       <c r="M176" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
@@ -11217,7 +11218,7 @@
         <v>315</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H177" s="1" t="s">
         <v>14</v>
@@ -11235,7 +11236,7 @@
         <v>9</v>
       </c>
       <c r="M177" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
@@ -11258,7 +11259,7 @@
         <v>315</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H178" s="1" t="s">
         <v>344</v>
@@ -11276,7 +11277,7 @@
         <v>23</v>
       </c>
       <c r="M178" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
@@ -11299,7 +11300,7 @@
         <v>315</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H179" s="1" t="s">
         <v>73</v>
@@ -11317,7 +11318,7 @@
         <v>9</v>
       </c>
       <c r="M179" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
@@ -11340,7 +11341,7 @@
         <v>315</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H180" s="1" t="s">
         <v>338</v>
@@ -11358,7 +11359,7 @@
         <v>23</v>
       </c>
       <c r="M180" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
@@ -11381,7 +11382,7 @@
         <v>315</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H181" s="1" t="s">
         <v>338</v>
@@ -11399,7 +11400,7 @@
         <v>9</v>
       </c>
       <c r="M181" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
@@ -11422,7 +11423,7 @@
         <v>315</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H182" s="1" t="s">
         <v>46</v>
@@ -11440,7 +11441,7 @@
         <v>23</v>
       </c>
       <c r="M182" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
@@ -11463,7 +11464,7 @@
         <v>315</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H183" s="1" t="s">
         <v>344</v>
@@ -11481,7 +11482,7 @@
         <v>23</v>
       </c>
       <c r="M183" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
@@ -11504,7 +11505,7 @@
         <v>315</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H184" s="1" t="s">
         <v>387</v>
@@ -11522,7 +11523,7 @@
         <v>23</v>
       </c>
       <c r="M184" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
@@ -11545,7 +11546,7 @@
         <v>315</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H185" s="1" t="s">
         <v>852</v>
@@ -11563,7 +11564,7 @@
         <v>23</v>
       </c>
       <c r="M185" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
@@ -11586,7 +11587,7 @@
         <v>315</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H186" s="9" t="s">
         <v>73</v>
@@ -11604,7 +11605,7 @@
         <v>9</v>
       </c>
       <c r="M186" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
@@ -11627,7 +11628,7 @@
         <v>315</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H187" s="9" t="s">
         <v>79</v>
@@ -11645,7 +11646,7 @@
         <v>23</v>
       </c>
       <c r="M187" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
@@ -11668,7 +11669,7 @@
         <v>315</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H188" s="9" t="s">
         <v>79</v>
@@ -11686,7 +11687,7 @@
         <v>23</v>
       </c>
       <c r="M188" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
@@ -11707,7 +11708,7 @@
         <v>315</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="H189" s="9" t="s">
         <v>79</v>
@@ -11725,7 +11726,7 @@
         <v>23</v>
       </c>
       <c r="M189" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
@@ -11748,7 +11749,7 @@
         <v>488</v>
       </c>
       <c r="G190" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="H190" s="1" t="s">
         <v>159</v>
@@ -11766,7 +11767,7 @@
         <v>9</v>
       </c>
       <c r="M190" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
@@ -11789,7 +11790,7 @@
         <v>488</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="H191" s="1" t="s">
         <v>381</v>
@@ -11807,7 +11808,7 @@
         <v>23</v>
       </c>
       <c r="M191" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
@@ -11830,7 +11831,7 @@
         <v>488</v>
       </c>
       <c r="G192" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="H192" s="1" t="s">
         <v>14</v>
@@ -11848,7 +11849,7 @@
         <v>23</v>
       </c>
       <c r="M192" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
@@ -11871,7 +11872,7 @@
         <v>488</v>
       </c>
       <c r="G193" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="H193" s="1" t="s">
         <v>344</v>
@@ -11889,7 +11890,7 @@
         <v>23</v>
       </c>
       <c r="M193" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
@@ -11912,7 +11913,7 @@
         <v>488</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="H194" s="1" t="s">
         <v>344</v>
@@ -11930,7 +11931,7 @@
         <v>23</v>
       </c>
       <c r="M194" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
@@ -11953,7 +11954,7 @@
         <v>488</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="H195" s="1" t="s">
         <v>381</v>
@@ -11971,7 +11972,7 @@
         <v>23</v>
       </c>
       <c r="M195" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
@@ -11994,7 +11995,7 @@
         <v>488</v>
       </c>
       <c r="G196" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="H196" s="1" t="s">
         <v>381</v>
@@ -12012,7 +12013,7 @@
         <v>23</v>
       </c>
       <c r="M196" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
@@ -12035,7 +12036,7 @@
         <v>488</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="H197" s="1" t="s">
         <v>338</v>
@@ -12053,7 +12054,7 @@
         <v>23</v>
       </c>
       <c r="M197" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.25">
@@ -12076,7 +12077,7 @@
         <v>488</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="H198" s="9" t="s">
         <v>908</v>
@@ -12094,7 +12095,7 @@
         <v>9</v>
       </c>
       <c r="M198" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
@@ -12117,7 +12118,7 @@
         <v>498</v>
       </c>
       <c r="G199" s="1" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="H199" s="1" t="s">
         <v>14</v>
@@ -12135,7 +12136,7 @@
         <v>9</v>
       </c>
       <c r="M199" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
@@ -12158,7 +12159,7 @@
         <v>498</v>
       </c>
       <c r="G200" s="1" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="H200" s="9" t="s">
         <v>73</v>
@@ -12176,7 +12177,7 @@
         <v>9</v>
       </c>
       <c r="M200" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
@@ -12199,7 +12200,7 @@
         <v>503</v>
       </c>
       <c r="G201" s="1" t="s">
-        <v>1041</v>
+        <v>1048</v>
       </c>
       <c r="H201" s="1" t="s">
         <v>79</v>
@@ -12217,7 +12218,7 @@
         <v>9</v>
       </c>
       <c r="M201" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
@@ -12240,7 +12241,7 @@
         <v>503</v>
       </c>
       <c r="G202" s="1" t="s">
-        <v>1041</v>
+        <v>1048</v>
       </c>
       <c r="H202" s="1" t="s">
         <v>46</v>
@@ -12258,7 +12259,7 @@
         <v>23</v>
       </c>
       <c r="M202" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
@@ -12281,7 +12282,7 @@
         <v>503</v>
       </c>
       <c r="G203" s="1" t="s">
-        <v>1041</v>
+        <v>1048</v>
       </c>
       <c r="H203" s="9" t="s">
         <v>46</v>
@@ -12299,7 +12300,7 @@
         <v>23</v>
       </c>
       <c r="M203" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
@@ -12322,7 +12323,7 @@
         <v>933</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H204" s="1" t="s">
         <v>327</v>
@@ -12340,7 +12341,7 @@
         <v>23</v>
       </c>
       <c r="M204" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
@@ -12363,7 +12364,7 @@
         <v>933</v>
       </c>
       <c r="G205" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H205" s="1" t="s">
         <v>20</v>
@@ -12381,7 +12382,7 @@
         <v>9</v>
       </c>
       <c r="M205" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.25">
@@ -12404,7 +12405,7 @@
         <v>933</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>338</v>
@@ -12422,7 +12423,7 @@
         <v>9</v>
       </c>
       <c r="M206" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
@@ -12445,7 +12446,7 @@
         <v>933</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>338</v>
@@ -12463,7 +12464,7 @@
         <v>23</v>
       </c>
       <c r="M207" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.25">
@@ -12486,7 +12487,7 @@
         <v>933</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H208" s="1" t="s">
         <v>79</v>
@@ -12504,7 +12505,7 @@
         <v>23</v>
       </c>
       <c r="M208" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.25">
@@ -12527,7 +12528,7 @@
         <v>933</v>
       </c>
       <c r="G209" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H209" s="1" t="s">
         <v>14</v>
@@ -12545,7 +12546,7 @@
         <v>23</v>
       </c>
       <c r="M209" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.25">
@@ -12568,7 +12569,7 @@
         <v>933</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H210" s="1" t="s">
         <v>452</v>
@@ -12586,7 +12587,7 @@
         <v>23</v>
       </c>
       <c r="M210" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">
@@ -12609,7 +12610,7 @@
         <v>933</v>
       </c>
       <c r="G211" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H211" s="1" t="s">
         <v>79</v>
@@ -12627,7 +12628,7 @@
         <v>23</v>
       </c>
       <c r="M211" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
@@ -12650,7 +12651,7 @@
         <v>933</v>
       </c>
       <c r="G212" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H212" s="1" t="s">
         <v>52</v>
@@ -12668,7 +12669,7 @@
         <v>9</v>
       </c>
       <c r="M212" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.25">
@@ -12691,7 +12692,7 @@
         <v>933</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H213" s="1" t="s">
         <v>106</v>
@@ -12709,7 +12710,7 @@
         <v>23</v>
       </c>
       <c r="M213" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.25">
@@ -12732,7 +12733,7 @@
         <v>933</v>
       </c>
       <c r="G214" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H214" s="1" t="s">
         <v>14</v>
@@ -12750,7 +12751,7 @@
         <v>9</v>
       </c>
       <c r="M214" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.25">
@@ -12773,7 +12774,7 @@
         <v>933</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H215" s="1" t="s">
         <v>381</v>
@@ -12791,7 +12792,7 @@
         <v>23</v>
       </c>
       <c r="M215" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
@@ -12814,7 +12815,7 @@
         <v>933</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H216" s="1" t="s">
         <v>79</v>
@@ -12832,7 +12833,7 @@
         <v>9</v>
       </c>
       <c r="M216" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
@@ -12855,7 +12856,7 @@
         <v>933</v>
       </c>
       <c r="G217" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H217" s="9" t="s">
         <v>73</v>
@@ -12873,7 +12874,7 @@
         <v>23</v>
       </c>
       <c r="M217" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">
@@ -12896,7 +12897,7 @@
         <v>933</v>
       </c>
       <c r="G218" s="1" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="H218" s="1" t="s">
         <v>73</v>
@@ -12914,7 +12915,7 @@
         <v>9</v>
       </c>
       <c r="M218" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.25">
@@ -12937,7 +12938,7 @@
         <v>992</v>
       </c>
       <c r="G219" s="1" t="s">
-        <v>1043</v>
+        <v>1038</v>
       </c>
       <c r="H219" s="9" t="s">
         <v>73</v>
@@ -12955,7 +12956,7 @@
         <v>23</v>
       </c>
       <c r="M219" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="220" spans="1:13" x14ac:dyDescent="0.25">
@@ -12978,7 +12979,7 @@
         <v>997</v>
       </c>
       <c r="G220" s="1" t="s">
-        <v>1044</v>
+        <v>1039</v>
       </c>
       <c r="H220" s="9" t="s">
         <v>79</v>
@@ -12996,7 +12997,7 @@
         <v>9</v>
       </c>
       <c r="M220" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="221" spans="1:13" x14ac:dyDescent="0.25">
@@ -13019,7 +13020,7 @@
         <v>1002</v>
       </c>
       <c r="G221" s="1" t="s">
-        <v>1045</v>
+        <v>1040</v>
       </c>
       <c r="H221" s="9" t="s">
         <v>73</v>
@@ -13037,7 +13038,7 @@
         <v>23</v>
       </c>
       <c r="M221" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.25">
@@ -13060,7 +13061,7 @@
         <v>1007</v>
       </c>
       <c r="G222" s="1" t="s">
-        <v>1046</v>
+        <v>1041</v>
       </c>
       <c r="H222" s="9" t="s">
         <v>452</v>
@@ -13078,7 +13079,7 @@
         <v>9</v>
       </c>
       <c r="M222" s="16" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
   </sheetData>
@@ -13087,10 +13088,15 @@
     <hyperlink ref="I60" r:id="rId2" xr:uid="{462FF499-1187-4F56-AF6A-38FE1932D72D}"/>
     <hyperlink ref="J60" r:id="rId3" xr:uid="{8140C1A1-133A-4695-BD17-342BDD42FD98}"/>
     <hyperlink ref="J17" r:id="rId4" xr:uid="{CEEEB50C-2987-4529-81E4-F5B63BC3D39B}"/>
+    <hyperlink ref="J37" r:id="rId5" xr:uid="{ED269723-3382-4BB4-8698-E6F36CC1043E}"/>
+    <hyperlink ref="J42" r:id="rId6" xr:uid="{CFE4EFB6-F946-414C-98DA-F38220B3F5A8}"/>
+    <hyperlink ref="J13" r:id="rId7" xr:uid="{90E7184A-F2D5-4D95-BFD5-83804B1605B5}"/>
+    <hyperlink ref="J20" r:id="rId8" xr:uid="{07CD7D82-2345-4BD3-8D89-1F555FCF44A0}"/>
+    <hyperlink ref="J31" r:id="rId9" xr:uid="{B3BDB410-1215-4B81-96B5-9B73166DCF23}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>